<commit_message>
Fix for ical file.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox/School/Teaching/DATA606 2021 Fall2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8347C2EC-2531-F143-A63D-7629EA304305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE515D2E-2173-CE43-A62B-4DF6D70F6072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14740" yWindow="9120" windowWidth="28800" windowHeight="17540" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
   <si>
     <t>Date</t>
   </si>
@@ -177,9 +177,6 @@
   </si>
   <si>
     <t>Intro to the Course</t>
-  </si>
-  <si>
-    <t>NO CLASS - Happy Thanksgiving</t>
   </si>
   <si>
     <t>TBD</t>
@@ -563,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA12B6D5-EAC3-1C40-AC8A-3C6A227098E4}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -615,7 +612,7 @@
         <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -816,20 +813,29 @@
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>44524</v>
+        <v>44531</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="E15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>44531</v>
+        <v>44538</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>7</v>
@@ -838,26 +844,9 @@
         <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>44538</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" t="s">
         <v>31</v>
       </c>
     </row>
@@ -945,7 +934,7 @@
         <v>44465</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
         <v>28</v>
@@ -1029,7 +1018,7 @@
         <v>44528</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated meetup page with link.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox (SPS)/Teaching/DATA606 2021 Fall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93295CC3-B8A1-BC40-B1B6-1AADA6FD76D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC39CCA4-2DF0-4D41-A87A-8FA7B913C007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14740" yWindow="9120" windowWidth="28800" windowHeight="17540" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="60">
   <si>
     <t>Date</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>[Recording and slides](/blog/meetup_05_foundation_for_inference/)</t>
+  </si>
+  <si>
+    <t>[Recording and slides](/blog/meetup_06_foundation_for_inference2/)</t>
   </si>
 </sst>
 </file>
@@ -586,7 +589,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -753,6 +756,9 @@
       </c>
       <c r="E8" t="s">
         <v>30</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Renumbered meetups to match chapters.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox (SPS)/Teaching/DATA606 2021 Fall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B3FF8C-0E25-4A42-BC13-57CB1B05B2C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F24508-079D-6242-9920-69822EEEE7AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14740" yWindow="9120" windowWidth="28800" windowHeight="17540" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
@@ -203,16 +203,16 @@
     <t>Chapter 8 - Linear Regression</t>
   </si>
   <si>
-    <t>[Recording and slides](/blog/meetup_05_foundation_for_inference/)</t>
-  </si>
-  <si>
-    <t>[Recording and slides](/blog/meetup_06_foundation_for_inference2/)</t>
-  </si>
-  <si>
-    <t>[Recording and slides](/blog/meetup_07_inference_for_categorical_data/)</t>
-  </si>
-  <si>
-    <t>[Recording and slides](/blog/meetup_08_inference_for_numerical_data/)</t>
+    <t>[Recording and slides](/blog/meetup_05a_foundation_for_inference/)</t>
+  </si>
+  <si>
+    <t>[Recording and slides](/blog/meetup_05b_foundation_for_inference2/)</t>
+  </si>
+  <si>
+    <t>[Recording and slides](/blog/meetup_06_inference_for_categorical_data/)</t>
+  </si>
+  <si>
+    <t>[Recording and slides](/blog/meetup_07_inference_for_numerical_data/)</t>
   </si>
 </sst>
 </file>
@@ -595,7 +595,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added link to meetup page.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox (SPS)/Teaching/DATA606 2021 Fall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F39C1D5-1099-C94C-A7C2-D7E41716EB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481FD767-BC7F-5E46-878B-3DAC7BB0D7DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14740" yWindow="9120" windowWidth="28800" windowHeight="17540" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
@@ -17,17 +17,26 @@
     <sheet name="Schedule" sheetId="2" r:id="rId2"/>
     <sheet name="Office_Hours" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="64">
   <si>
     <t>Date</t>
   </si>
@@ -216,6 +225,9 @@
   </si>
   <si>
     <t>[Recording and slides](/blog/meetup_08_linear_regression1/)</t>
+  </si>
+  <si>
+    <t>[Recording and slides](/blog/meetup_08b_linear_regression2/)</t>
   </si>
 </sst>
 </file>
@@ -598,7 +610,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -845,6 +857,9 @@
       </c>
       <c r="E12" t="s">
         <v>30</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>